<commit_message>
Multile Data Data Added in ORG Test.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{07F7BF30-85F4-44CA-9E9D-BE37DBDD0EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{402A47D9-4F12-4444-AD84-0256F3D4F579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ProductData" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M13"/>
+  <oleSize ref="A1:S13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="85">
   <si>
     <t>TC_ID</t>
   </si>
@@ -265,13 +265,31 @@
   </si>
   <si>
     <t>Mr.</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>Electronics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +317,17 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
@@ -363,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -381,6 +410,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590B7557-1150-4C90-BF4A-2C91F83F8663}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -992,15 +1023,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAAEFBF-0003-4C1C-934E-6C3A3B4F37D9}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="122" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1049,6 +1080,30 @@
       </c>
       <c r="B6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>